<commit_message>
Fixed add author's saved state issue
</commit_message>
<xml_diff>
--- a/Pacakges.xlsx
+++ b/Pacakges.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17870"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Dev\ReactLearn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Reactjs\ReactLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Backlog" sheetId="2" r:id="rId1"/>
+    <sheet name="Packages" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="77">
   <si>
     <t>seamless-immutable</t>
   </si>
@@ -162,13 +163,106 @@
   </si>
   <si>
     <t>request-promise</t>
+  </si>
+  <si>
+    <t>10. Revert abandoned changes</t>
+  </si>
+  <si>
+    <t>12. add Delete icon</t>
+  </si>
+  <si>
+    <t>13. Styling</t>
+  </si>
+  <si>
+    <t>13. Radium pacakge for stylying</t>
+  </si>
+  <si>
+    <t>14. SAAS</t>
+  </si>
+  <si>
+    <t>15. reselect</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Satus</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>11. Pagination</t>
+  </si>
+  <si>
+    <t>Handle 404 on manage course page</t>
+  </si>
+  <si>
+    <t>Author Adminstration (cant delete a author if he/she has a course)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Course  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide empty course list when all course are deleted  </t>
+  </si>
+  <si>
+    <t>Client side validation for category and link data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show #course on header  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort course table (mapStateToProps)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirmation dialouge on delete  </t>
+  </si>
+  <si>
+    <t>Unsaved changes message when user is leaving manage course page</t>
+  </si>
+  <si>
+    <t>Modal page</t>
+  </si>
+  <si>
+    <t>Router redirect</t>
+  </si>
+  <si>
+    <t>Styling of react components</t>
+  </si>
+  <si>
+    <t>Default Sorting on page load</t>
+  </si>
+  <si>
+    <t>Add DOB with date control in Add author page</t>
+  </si>
+  <si>
+    <t>Add a date of course update/add</t>
+  </si>
+  <si>
+    <t>Add a course description page</t>
+  </si>
+  <si>
+    <t>Add course review</t>
+  </si>
+  <si>
+    <t>Add Course level</t>
+  </si>
+  <si>
+    <t>Saving author functionality</t>
+  </si>
+  <si>
+    <t>Delete author with own delete icon</t>
+  </si>
+  <si>
+    <t>Restruture Course module</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,13 +284,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -212,7 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -222,6 +330,8 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -537,10 +647,241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:D37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="68" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" activeCellId="1" sqref="C5:C55 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,182 +891,253 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C6" s="6"/>
       <c r="D6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C7" s="6"/>
       <c r="D7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C8" s="6"/>
       <c r="D8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="6"/>
       <c r="D9" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C10" s="6"/>
+    </row>
     <row r="11" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C12" s="6"/>
       <c r="D12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C13" s="6"/>
       <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C14" s="6"/>
       <c r="D14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C15" s="6"/>
       <c r="D15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C16" s="6"/>
       <c r="D16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="6"/>
       <c r="D17" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="6"/>
       <c r="D18" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="6"/>
       <c r="D19" s="3" t="s">
         <v>44</v>
       </c>
     </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="6"/>
+    </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
+      <c r="C21" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" s="6"/>
       <c r="D22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23" s="6"/>
       <c r="D23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C24" s="6"/>
       <c r="D24" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C26" s="6"/>
+    </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
+      <c r="C27" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C28" s="6"/>
       <c r="D28" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C30" s="6"/>
+    </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
+      <c r="C31" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C32" s="6"/>
       <c r="D32" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C34" s="6"/>
+    </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C35" t="s">
+      <c r="C35" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C36" s="6"/>
       <c r="D36" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C37" s="6"/>
       <c r="D37" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C38" s="6"/>
       <c r="D38" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C40" s="6"/>
+    </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
+      <c r="C41" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C42" s="6"/>
       <c r="D42" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C43" s="6"/>
       <c r="D43" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C44" s="6"/>
       <c r="D44" s="3" t="s">
         <v>45</v>
       </c>
     </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C45" s="6"/>
+    </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C46" t="s">
+      <c r="C46" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C47" s="6"/>
       <c r="D47" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C48" s="6"/>
       <c r="D48" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C50" s="6"/>
+    </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C51" t="s">
+      <c r="C51" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C52" s="6"/>
       <c r="D52" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C54" s="6"/>
+    </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
+      <c r="C55" s="6" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>